<commit_message>
actualizacao 17h dia 15 de janeiro
</commit_message>
<xml_diff>
--- a/Data/indiv_PI.xlsx
+++ b/Data/indiv_PI.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -410,14 +410,19 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Sessao 1</t>
+        </is>
+      </c>
       <c r="E2">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -438,17 +443,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E3">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F3">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -469,17 +474,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <v>13</v>
       </c>
       <c r="G4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -500,17 +505,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -526,22 +531,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -560,14 +565,19 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sessao 2</t>
+        </is>
+      </c>
       <c r="E7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -588,17 +598,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -619,17 +629,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -640,27 +650,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CARAPIRA</t>
+          <t>MARINGUE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Sessao 3</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="E10">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -671,27 +676,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CARAPIRA</t>
+          <t>MARINGUE</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
@@ -710,14 +715,19 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Sessao 2</t>
+        </is>
+      </c>
       <c r="E12">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F12">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G12">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -738,17 +748,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E13">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="F13">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G13">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
@@ -764,22 +774,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>FEMININO</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Sessao 2</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="E14">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="F14">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G14">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -795,22 +800,22 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E15">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -829,14 +834,19 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Sessao 2</t>
+        </is>
+      </c>
       <c r="E16">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G16">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -857,17 +867,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E17">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F17">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
@@ -878,27 +888,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MARINGUE</t>
+          <t>NACOLOLO</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Sessao 2</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="E18">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -909,27 +914,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MARINGUE</t>
+          <t>NACOLOLO</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
@@ -940,27 +945,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MARINGUE</t>
+          <t>NACOLOLO</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E20">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -979,14 +984,19 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sessao 3</t>
+        </is>
+      </c>
       <c r="E21">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F21">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G21">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22">
@@ -1007,17 +1017,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E22">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1033,22 +1043,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>FEMININO</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Sessao 2</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="E23">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="F23">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G23">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1064,22 +1069,22 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E24">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F24">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G24">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -1095,22 +1100,22 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G25">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
@@ -1129,14 +1134,19 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Sessao 3</t>
+        </is>
+      </c>
       <c r="E26">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G26">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
@@ -1147,12 +1157,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>NACOLOLO</t>
+          <t>NAPALA</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1161,13 +1171,13 @@
         </is>
       </c>
       <c r="E27">
+        <v>27</v>
+      </c>
+      <c r="F27">
         <v>12</v>
       </c>
-      <c r="F27">
-        <v>4</v>
-      </c>
       <c r="G27">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
@@ -1178,12 +1188,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>NACOLOLO</t>
+          <t>NAPALA</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1192,13 +1202,13 @@
         </is>
       </c>
       <c r="E28">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F28">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G28">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29">
@@ -1209,27 +1219,27 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NACOLOLO</t>
+          <t>NAPALA</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E29">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1240,7 +1250,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>NACOLOLO</t>
+          <t>NAPALA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1250,17 +1260,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31">
@@ -1271,7 +1281,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>NACOLOLO</t>
+          <t>NAPALA</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1281,17 +1291,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Sessao 5</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
@@ -1307,17 +1317,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E32">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1328,7 +1343,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1336,19 +1351,14 @@
           <t>FEMININO</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Sessao 1</t>
-        </is>
-      </c>
       <c r="E33">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="F33">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -1359,7 +1369,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1369,17 +1379,17 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E34">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F34">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G34">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
@@ -1390,7 +1400,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1400,17 +1410,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E35">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F35">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G35">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36">
@@ -1421,7 +1431,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1431,17 +1441,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E36">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F36">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G36">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1452,22 +1462,27 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E37">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="F37">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G37">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1478,7 +1493,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1486,19 +1501,14 @@
           <t>MASCULINO</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Sessao 1</t>
-        </is>
-      </c>
       <c r="E38">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G38">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
@@ -1509,7 +1519,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1519,17 +1529,17 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E39">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G39">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
@@ -1540,7 +1550,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1550,14 +1560,14 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E40">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F40">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G40">
         <v>11</v>
@@ -1571,7 +1581,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>NAPALA</t>
+          <t>TAPALALA</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1581,17 +1591,17 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E41">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F41">
         <v>5</v>
       </c>
       <c r="G41">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1607,28 +1617,33 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E42">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F42">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1636,30 +1651,25 @@
           <t>FEMININO</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Sessao 1</t>
-        </is>
-      </c>
       <c r="E43">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F43">
+        <v>16</v>
+      </c>
+      <c r="G43">
         <v>9</v>
-      </c>
-      <c r="G43">
-        <v>12</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1669,28 +1679,28 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E44">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F44">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G44">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1700,28 +1710,28 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E45">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F45">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G45">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1731,14 +1741,14 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E46">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G46">
         <v>9</v>
@@ -1747,12 +1757,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1762,28 +1772,28 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Sessao 5</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E47">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1792,24 +1802,24 @@
         </is>
       </c>
       <c r="E48">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F48">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G48">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1823,24 +1833,24 @@
         </is>
       </c>
       <c r="E49">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F49">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G49">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1854,24 +1864,24 @@
         </is>
       </c>
       <c r="E50">
+        <v>28</v>
+      </c>
+      <c r="F50">
         <v>20</v>
       </c>
-      <c r="F50">
-        <v>10</v>
-      </c>
       <c r="G50">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1885,24 +1895,24 @@
         </is>
       </c>
       <c r="E51">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F51">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G51">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>1º DE MAIO</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1919,41 +1929,36 @@
         <v>3</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MONAPO</t>
+          <t>RIBAUE</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>TAPALALA</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Sessao 5</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54">
@@ -1964,7 +1969,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1972,14 +1977,19 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Sessao 1</t>
+        </is>
+      </c>
       <c r="E54">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F54">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G54">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55">
@@ -1990,7 +2000,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2000,17 +2010,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E55">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F55">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G55">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56">
@@ -2021,7 +2031,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2031,17 +2041,17 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G56">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57">
@@ -2052,7 +2062,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2062,17 +2072,17 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E57">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F57">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
@@ -2083,27 +2093,22 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>FEMININO</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Sessao 4</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="E58">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F58">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G58">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59">
@@ -2114,27 +2119,27 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Sessao 5</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60">
@@ -2145,7 +2150,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2153,14 +2158,19 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Sessao 2</t>
+        </is>
+      </c>
       <c r="E60">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F60">
+        <v>6</v>
+      </c>
+      <c r="G60">
         <v>10</v>
-      </c>
-      <c r="G60">
-        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -2171,7 +2181,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2181,17 +2191,17 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E61">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F61">
         <v>8</v>
       </c>
       <c r="G61">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62">
@@ -2202,7 +2212,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>CUNLE SEDE</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2212,17 +2222,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E62">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="G62">
         <v>6</v>
-      </c>
-      <c r="G62">
-        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -2233,27 +2243,27 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E63">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F63">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G63">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64">
@@ -2264,27 +2274,27 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1º DE MAIO</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E64">
+        <v>17</v>
+      </c>
+      <c r="F64">
         <v>10</v>
       </c>
-      <c r="F64">
-        <v>2</v>
-      </c>
       <c r="G64">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65">
@@ -2295,7 +2305,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2303,14 +2313,19 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Sessao 3</t>
+        </is>
+      </c>
       <c r="E65">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G65">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -2321,7 +2336,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2331,17 +2346,17 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 5</t>
         </is>
       </c>
       <c r="E66">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G66">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -2352,7 +2367,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2362,17 +2377,17 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 6</t>
         </is>
       </c>
       <c r="E67">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F67">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G67">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -2383,27 +2398,27 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E68">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G68">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69">
@@ -2414,27 +2429,27 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>FEMININO</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E69">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F69">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G69">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70">
@@ -2445,7 +2460,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2453,14 +2468,19 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Sessao 3</t>
+        </is>
+      </c>
       <c r="E70">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="F70">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G70">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71">
@@ -2471,7 +2491,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2481,17 +2501,17 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E71">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F71">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2502,7 +2522,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2512,17 +2532,17 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 5</t>
         </is>
       </c>
       <c r="E72">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F72">
         <v>2</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -2533,7 +2553,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>MARROCANE</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2543,14 +2563,14 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 6</t>
         </is>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G73">
         <v>2</v>
@@ -2564,27 +2584,27 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>CUNLE SEDE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>MASCULINO</t>
+          <t>FEMININO</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 1</t>
         </is>
       </c>
       <c r="E74">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F74">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="G74">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75">
@@ -2595,7 +2615,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2603,14 +2623,19 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Sessao 2</t>
+        </is>
+      </c>
       <c r="E75">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F75">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G75">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76">
@@ -2621,7 +2646,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2631,17 +2656,17 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E76">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F76">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G76">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77">
@@ -2652,7 +2677,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2662,17 +2687,17 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E77">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="F77">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G77">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78">
@@ -2683,7 +2708,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2693,17 +2718,17 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 5</t>
         </is>
       </c>
       <c r="E78">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F78">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G78">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -2714,7 +2739,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2724,17 +2749,17 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 6</t>
         </is>
       </c>
       <c r="E79">
+        <v>8</v>
+      </c>
+      <c r="F79">
         <v>7</v>
       </c>
-      <c r="F79">
-        <v>3</v>
-      </c>
       <c r="G79">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -2745,7 +2770,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2753,14 +2778,19 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Sessao 1</t>
+        </is>
+      </c>
       <c r="E80">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F80">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G80">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81">
@@ -2771,7 +2801,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2781,17 +2811,17 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Sessao 1</t>
+          <t>Sessao 2</t>
         </is>
       </c>
       <c r="E81">
+        <v>23</v>
+      </c>
+      <c r="F81">
         <v>12</v>
       </c>
-      <c r="F81">
-        <v>5</v>
-      </c>
       <c r="G81">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82">
@@ -2802,7 +2832,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2812,17 +2842,17 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Sessao 2</t>
+          <t>Sessao 3</t>
         </is>
       </c>
       <c r="E82">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F82">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G82">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83">
@@ -2833,7 +2863,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2843,17 +2873,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Sessao 3</t>
+          <t>Sessao 4</t>
         </is>
       </c>
       <c r="E83">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F83">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G83">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84">
@@ -2864,7 +2894,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2874,17 +2904,17 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Sessao 4</t>
+          <t>Sessao 5</t>
         </is>
       </c>
       <c r="E84">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F84">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G84">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2895,7 +2925,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>MARROCANE</t>
+          <t>NACHILAPA</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2905,317 +2935,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Sessao 5</t>
+          <t>Sessao 6</t>
         </is>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G85">
         <v>1</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>FEMININO</t>
-        </is>
-      </c>
-      <c r="E86">
-        <v>23</v>
-      </c>
-      <c r="F86">
-        <v>20</v>
-      </c>
-      <c r="G86">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>FEMININO</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>Sessao 1</t>
-        </is>
-      </c>
-      <c r="E87">
-        <v>27</v>
-      </c>
-      <c r="F87">
-        <v>10</v>
-      </c>
-      <c r="G87">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>FEMININO</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>Sessao 2</t>
-        </is>
-      </c>
-      <c r="E88">
-        <v>26</v>
-      </c>
-      <c r="F88">
-        <v>11</v>
-      </c>
-      <c r="G88">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>FEMININO</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>Sessao 3</t>
-        </is>
-      </c>
-      <c r="E89">
-        <v>17</v>
-      </c>
-      <c r="F89">
-        <v>9</v>
-      </c>
-      <c r="G89">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>FEMININO</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Sessao 4</t>
-        </is>
-      </c>
-      <c r="E90">
-        <v>8</v>
-      </c>
-      <c r="F90">
-        <v>2</v>
-      </c>
-      <c r="G90">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>MASCULINO</t>
-        </is>
-      </c>
-      <c r="E91">
-        <v>7</v>
-      </c>
-      <c r="F91">
-        <v>4</v>
-      </c>
-      <c r="G91">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>MASCULINO</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>Sessao 1</t>
-        </is>
-      </c>
-      <c r="E92">
-        <v>20</v>
-      </c>
-      <c r="F92">
-        <v>9</v>
-      </c>
-      <c r="G92">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>MASCULINO</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>Sessao 2</t>
-        </is>
-      </c>
-      <c r="E93">
-        <v>20</v>
-      </c>
-      <c r="F93">
-        <v>9</v>
-      </c>
-      <c r="G93">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>MASCULINO</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>Sessao 3</t>
-        </is>
-      </c>
-      <c r="E94">
-        <v>19</v>
-      </c>
-      <c r="F94">
-        <v>11</v>
-      </c>
-      <c r="G94">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>RIBAUE</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>NACHILAPA</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>MASCULINO</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Sessao 4</t>
-        </is>
-      </c>
-      <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95">
-        <v>1</v>
-      </c>
-      <c r="G95">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacao da Sessao PI 9 e AG 6
</commit_message>
<xml_diff>
--- a/Data/indiv_PI.xlsx
+++ b/Data/indiv_PI.xlsx
@@ -416,13 +416,13 @@
         </is>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G2">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -447,13 +447,13 @@
         </is>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F3">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G3">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="E4">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
@@ -509,13 +509,13 @@
         </is>
       </c>
       <c r="E5">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F5">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G5">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -540,13 +540,13 @@
         </is>
       </c>
       <c r="E6">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="F6">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G6">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
@@ -571,13 +571,13 @@
         </is>
       </c>
       <c r="E7">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F7">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -608,7 +608,7 @@
         <v>23</v>
       </c>
       <c r="G8">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -633,13 +633,13 @@
         </is>
       </c>
       <c r="E9">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F9">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G9">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
@@ -664,13 +664,13 @@
         </is>
       </c>
       <c r="E10">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F10">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G10">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
@@ -695,13 +695,13 @@
         </is>
       </c>
       <c r="E11">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F11">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G11">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -726,13 +726,13 @@
         </is>
       </c>
       <c r="E12">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G12">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -757,13 +757,13 @@
         </is>
       </c>
       <c r="E13">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G13">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -788,13 +788,13 @@
         </is>
       </c>
       <c r="E14">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F14">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G14">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
@@ -819,13 +819,13 @@
         </is>
       </c>
       <c r="E15">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F15">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G15">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -850,13 +850,13 @@
         </is>
       </c>
       <c r="E16">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F16">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G16">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -887,7 +887,7 @@
         <v>14</v>
       </c>
       <c r="G17">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="E18">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F18">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G18">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -943,13 +943,13 @@
         </is>
       </c>
       <c r="E19">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19">
         <v>14</v>
-      </c>
-      <c r="G19">
-        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -974,13 +974,13 @@
         </is>
       </c>
       <c r="E20">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G20">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -1005,10 +1005,10 @@
         </is>
       </c>
       <c r="E21">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F21">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G21">
         <v>23</v>
@@ -1036,13 +1036,13 @@
         </is>
       </c>
       <c r="E22">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F22">
         <v>13</v>
       </c>
       <c r="G22">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
@@ -1067,13 +1067,13 @@
         </is>
       </c>
       <c r="E23">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F23">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G23">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -1098,13 +1098,13 @@
         </is>
       </c>
       <c r="E24">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F24">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G24">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
@@ -1129,13 +1129,13 @@
         </is>
       </c>
       <c r="E25">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
@@ -1160,13 +1160,13 @@
         </is>
       </c>
       <c r="E26">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F26">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G26">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27">
@@ -1191,13 +1191,13 @@
         </is>
       </c>
       <c r="E27">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F27">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G27">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28">
@@ -1222,10 +1222,10 @@
         </is>
       </c>
       <c r="E28">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F28">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G28">
         <v>22</v>
@@ -1253,10 +1253,10 @@
         </is>
       </c>
       <c r="E29">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G29">
         <v>17</v>
@@ -1284,13 +1284,13 @@
         </is>
       </c>
       <c r="E30">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F30">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G30">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
@@ -1315,10 +1315,10 @@
         </is>
       </c>
       <c r="E31">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G31">
         <v>17</v>
@@ -1346,13 +1346,13 @@
         </is>
       </c>
       <c r="E32">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G32">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33">
@@ -1377,10 +1377,10 @@
         </is>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G33">
         <v>17</v>
@@ -1411,10 +1411,10 @@
         <v>23</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G34">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35">
@@ -1439,13 +1439,13 @@
         </is>
       </c>
       <c r="E35">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G35">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36">
@@ -1470,13 +1470,13 @@
         </is>
       </c>
       <c r="E36">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G36">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37">
@@ -1501,13 +1501,13 @@
         </is>
       </c>
       <c r="E37">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F37">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G37">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38">
@@ -1532,13 +1532,13 @@
         </is>
       </c>
       <c r="E38">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F38">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G38">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39">
@@ -1563,13 +1563,13 @@
         </is>
       </c>
       <c r="E39">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F39">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G39">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40">
@@ -1594,13 +1594,13 @@
         </is>
       </c>
       <c r="E40">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F40">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G40">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41">
@@ -1625,13 +1625,13 @@
         </is>
       </c>
       <c r="E41">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F41">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G41">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42">
@@ -1656,13 +1656,13 @@
         </is>
       </c>
       <c r="E42">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F42">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G42">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43">
@@ -1687,13 +1687,13 @@
         </is>
       </c>
       <c r="E43">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F43">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G43">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44">
@@ -1721,10 +1721,10 @@
         <v>35</v>
       </c>
       <c r="F44">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G44">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45">
@@ -1749,13 +1749,13 @@
         </is>
       </c>
       <c r="E45">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F45">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G45">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46">
@@ -1780,13 +1780,13 @@
         </is>
       </c>
       <c r="E46">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F46">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G46">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47">
@@ -1811,13 +1811,13 @@
         </is>
       </c>
       <c r="E47">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F47">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G47">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48">
@@ -1842,13 +1842,13 @@
         </is>
       </c>
       <c r="E48">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F48">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G48">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49">
@@ -1873,13 +1873,13 @@
         </is>
       </c>
       <c r="E49">
+        <v>27</v>
+      </c>
+      <c r="F49">
+        <v>8</v>
+      </c>
+      <c r="G49">
         <v>19</v>
-      </c>
-      <c r="F49">
-        <v>9</v>
-      </c>
-      <c r="G49">
-        <v>10</v>
       </c>
     </row>
     <row r="50">
@@ -1904,13 +1904,13 @@
         </is>
       </c>
       <c r="E50">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F50">
         <v>8</v>
       </c>
       <c r="G50">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51">
@@ -1935,13 +1935,13 @@
         </is>
       </c>
       <c r="E51">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F51">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G51">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52">
@@ -1966,13 +1966,13 @@
         </is>
       </c>
       <c r="E52">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F52">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G52">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53">
@@ -1997,13 +1997,13 @@
         </is>
       </c>
       <c r="E53">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F53">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G53">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54">
@@ -2028,10 +2028,10 @@
         </is>
       </c>
       <c r="E54">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F54">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G54">
         <v>18</v>
@@ -2059,13 +2059,13 @@
         </is>
       </c>
       <c r="E55">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F55">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G55">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56">
@@ -2090,13 +2090,13 @@
         </is>
       </c>
       <c r="E56">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F56">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G56">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57">
@@ -2121,13 +2121,13 @@
         </is>
       </c>
       <c r="E57">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F57">
         <v>16</v>
       </c>
       <c r="G57">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58">
@@ -2152,13 +2152,13 @@
         </is>
       </c>
       <c r="E58">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F58">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G58">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59">
@@ -2183,13 +2183,13 @@
         </is>
       </c>
       <c r="E59">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F59">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G59">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60">
@@ -2214,10 +2214,10 @@
         </is>
       </c>
       <c r="E60">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F60">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G60">
         <v>25</v>
@@ -2245,13 +2245,13 @@
         </is>
       </c>
       <c r="E61">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F61">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G61">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62">
@@ -2276,13 +2276,13 @@
         </is>
       </c>
       <c r="E62">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F62">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G62">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63">
@@ -2307,10 +2307,10 @@
         </is>
       </c>
       <c r="E63">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F63">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G63">
         <v>23</v>
@@ -2338,13 +2338,13 @@
         </is>
       </c>
       <c r="E64">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F64">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G64">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65">
@@ -2369,13 +2369,13 @@
         </is>
       </c>
       <c r="E65">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G65">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66">
@@ -2400,13 +2400,13 @@
         </is>
       </c>
       <c r="E66">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F66">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G66">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -2431,13 +2431,13 @@
         </is>
       </c>
       <c r="E67">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F67">
         <v>4</v>
       </c>
       <c r="G67">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68">
@@ -2462,13 +2462,13 @@
         </is>
       </c>
       <c r="E68">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F68">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G68">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69">
@@ -2496,10 +2496,10 @@
         <v>12</v>
       </c>
       <c r="F69">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G69">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70">
@@ -2524,13 +2524,13 @@
         </is>
       </c>
       <c r="E70">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F70">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G70">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71">
@@ -2555,13 +2555,13 @@
         </is>
       </c>
       <c r="E71">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F71">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G71">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72">
@@ -2586,13 +2586,13 @@
         </is>
       </c>
       <c r="E72">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F72">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G72">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73">
@@ -2617,13 +2617,13 @@
         </is>
       </c>
       <c r="E73">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F73">
         <v>3</v>
       </c>
       <c r="G73">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74">
@@ -2648,13 +2648,13 @@
         </is>
       </c>
       <c r="E74">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F74">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G74">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75">
@@ -2679,13 +2679,13 @@
         </is>
       </c>
       <c r="E75">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F75">
         <v>23</v>
       </c>
       <c r="G75">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76">
@@ -2710,13 +2710,13 @@
         </is>
       </c>
       <c r="E76">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F76">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G76">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77">
@@ -2741,13 +2741,13 @@
         </is>
       </c>
       <c r="E77">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F77">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G77">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78">
@@ -2772,13 +2772,13 @@
         </is>
       </c>
       <c r="E78">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F78">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G78">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79">
@@ -2803,13 +2803,13 @@
         </is>
       </c>
       <c r="E79">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F79">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G79">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80">
@@ -2834,10 +2834,10 @@
         </is>
       </c>
       <c r="E80">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F80">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G80">
         <v>16</v>
@@ -2865,13 +2865,13 @@
         </is>
       </c>
       <c r="E81">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F81">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G81">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82">
@@ -2896,13 +2896,13 @@
         </is>
       </c>
       <c r="E82">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F82">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G82">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83">
@@ -2927,10 +2927,10 @@
         </is>
       </c>
       <c r="E83">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F83">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G83">
         <v>19</v>
@@ -2958,13 +2958,13 @@
         </is>
       </c>
       <c r="E84">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F84">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G84">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85">
@@ -2989,13 +2989,13 @@
         </is>
       </c>
       <c r="E85">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F85">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G85">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86">
@@ -3020,10 +3020,10 @@
         </is>
       </c>
       <c r="E86">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F86">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G86">
         <v>18</v>
@@ -3051,10 +3051,10 @@
         </is>
       </c>
       <c r="E87">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F87">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G87">
         <v>18</v>
@@ -3082,13 +3082,13 @@
         </is>
       </c>
       <c r="E88">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F88">
         <v>6</v>
       </c>
       <c r="G88">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89">
@@ -3113,13 +3113,13 @@
         </is>
       </c>
       <c r="E89">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F89">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G89">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90">
@@ -3144,13 +3144,13 @@
         </is>
       </c>
       <c r="E90">
+        <v>25</v>
+      </c>
+      <c r="F90">
+        <v>7</v>
+      </c>
+      <c r="G90">
         <v>18</v>
-      </c>
-      <c r="F90">
-        <v>5</v>
-      </c>
-      <c r="G90">
-        <v>13</v>
       </c>
     </row>
     <row r="91">
@@ -3175,13 +3175,13 @@
         </is>
       </c>
       <c r="E91">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F91">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G91">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92">
@@ -3206,13 +3206,13 @@
         </is>
       </c>
       <c r="E92">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F92">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G92">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93">
@@ -3237,13 +3237,13 @@
         </is>
       </c>
       <c r="E93">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F93">
         <v>9</v>
       </c>
       <c r="G93">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94">
@@ -3271,10 +3271,10 @@
         <v>23</v>
       </c>
       <c r="F94">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G94">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95">
@@ -3299,13 +3299,13 @@
         </is>
       </c>
       <c r="E95">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F95">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G95">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96">
@@ -3330,13 +3330,13 @@
         </is>
       </c>
       <c r="E96">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F96">
         <v>8</v>
       </c>
       <c r="G96">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97">
@@ -3361,13 +3361,13 @@
         </is>
       </c>
       <c r="E97">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F97">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G97">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98">
@@ -3392,13 +3392,13 @@
         </is>
       </c>
       <c r="E98">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F98">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G98">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99">
@@ -3423,13 +3423,13 @@
         </is>
       </c>
       <c r="E99">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F99">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G99">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100">
@@ -3454,13 +3454,13 @@
         </is>
       </c>
       <c r="E100">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F100">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G100">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101">
@@ -3485,13 +3485,13 @@
         </is>
       </c>
       <c r="E101">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F101">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G101">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102">
@@ -3516,13 +3516,13 @@
         </is>
       </c>
       <c r="E102">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F102">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G102">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103">
@@ -3547,13 +3547,13 @@
         </is>
       </c>
       <c r="E103">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F103">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G103">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104">
@@ -3578,13 +3578,13 @@
         </is>
       </c>
       <c r="E104">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F104">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G104">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105">
@@ -3609,13 +3609,13 @@
         </is>
       </c>
       <c r="E105">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F105">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G105">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106">
@@ -3640,10 +3640,10 @@
         </is>
       </c>
       <c r="E106">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F106">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G106">
         <v>11</v>
@@ -3677,7 +3677,7 @@
         <v>6</v>
       </c>
       <c r="G107">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108">
@@ -3705,10 +3705,10 @@
         <v>19</v>
       </c>
       <c r="F108">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G108">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109">
@@ -3733,13 +3733,13 @@
         </is>
       </c>
       <c r="E109">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F109">
         <v>9</v>
       </c>
       <c r="G109">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110">
@@ -3764,13 +3764,13 @@
         </is>
       </c>
       <c r="E110">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F110">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G110">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111">
@@ -3795,13 +3795,13 @@
         </is>
       </c>
       <c r="E111">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F111">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G111">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112">
@@ -3826,13 +3826,13 @@
         </is>
       </c>
       <c r="E112">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F112">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G112">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113">
@@ -3857,13 +3857,13 @@
         </is>
       </c>
       <c r="E113">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F113">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G113">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114">
@@ -3888,13 +3888,13 @@
         </is>
       </c>
       <c r="E114">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F114">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G114">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="115">
@@ -3919,13 +3919,13 @@
         </is>
       </c>
       <c r="E115">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F115">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G115">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116">
@@ -3950,13 +3950,13 @@
         </is>
       </c>
       <c r="E116">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F116">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G116">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117">
@@ -3981,13 +3981,13 @@
         </is>
       </c>
       <c r="E117">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F117">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G117">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118">
@@ -4012,13 +4012,13 @@
         </is>
       </c>
       <c r="E118">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F118">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G118">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119">
@@ -4043,10 +4043,10 @@
         </is>
       </c>
       <c r="E119">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F119">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G119">
         <v>8</v>
@@ -4074,13 +4074,13 @@
         </is>
       </c>
       <c r="E120">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F120">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G120">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121">
@@ -4105,13 +4105,13 @@
         </is>
       </c>
       <c r="E121">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F121">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G121">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122">
@@ -4139,10 +4139,10 @@
         <v>21</v>
       </c>
       <c r="F122">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G122">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123">
@@ -4167,13 +4167,13 @@
         </is>
       </c>
       <c r="E123">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F123">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G123">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124">
@@ -4198,13 +4198,13 @@
         </is>
       </c>
       <c r="E124">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F124">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G124">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125">
@@ -4229,13 +4229,13 @@
         </is>
       </c>
       <c r="E125">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F125">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G125">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126">
@@ -4260,13 +4260,13 @@
         </is>
       </c>
       <c r="E126">
+        <v>24</v>
+      </c>
+      <c r="F126">
         <v>18</v>
       </c>
-      <c r="F126">
-        <v>13</v>
-      </c>
       <c r="G126">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127">
@@ -4291,13 +4291,13 @@
         </is>
       </c>
       <c r="E127">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F127">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G127">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128">
@@ -4325,10 +4325,10 @@
         <v>7</v>
       </c>
       <c r="F128">
+        <v>3</v>
+      </c>
+      <c r="G128">
         <v>4</v>
-      </c>
-      <c r="G128">
-        <v>3</v>
       </c>
     </row>
     <row r="129">
@@ -4353,10 +4353,10 @@
         </is>
       </c>
       <c r="E129">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F129">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G129">
         <v>3</v>
@@ -4387,10 +4387,10 @@
         <v>8</v>
       </c>
       <c r="F130">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G130">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131">
@@ -4415,13 +4415,13 @@
         </is>
       </c>
       <c r="E131">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F131">
+        <v>5</v>
+      </c>
+      <c r="G131">
         <v>3</v>
-      </c>
-      <c r="G131">
-        <v>4</v>
       </c>
     </row>
     <row r="132">
@@ -4446,13 +4446,13 @@
         </is>
       </c>
       <c r="E132">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F132">
+        <v>1</v>
+      </c>
+      <c r="G132">
         <v>4</v>
-      </c>
-      <c r="G132">
-        <v>2</v>
       </c>
     </row>
     <row r="133">
@@ -4508,10 +4508,10 @@
         </is>
       </c>
       <c r="E134">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F134">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G134">
         <v>4</v>
@@ -4539,10 +4539,10 @@
         </is>
       </c>
       <c r="E135">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F135">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G135">
         <v>3</v>
@@ -4570,13 +4570,13 @@
         </is>
       </c>
       <c r="E136">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F136">
         <v>4</v>
       </c>
       <c r="G136">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137">
@@ -4601,13 +4601,13 @@
         </is>
       </c>
       <c r="E137">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F137">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G137">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138">
@@ -4632,10 +4632,10 @@
         </is>
       </c>
       <c r="E138">
+        <v>16</v>
+      </c>
+      <c r="F138">
         <v>12</v>
-      </c>
-      <c r="F138">
-        <v>8</v>
       </c>
       <c r="G138">
         <v>4</v>
@@ -4663,10 +4663,10 @@
         </is>
       </c>
       <c r="E139">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F139">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G139">
         <v>5</v>
@@ -4694,10 +4694,10 @@
         </is>
       </c>
       <c r="E140">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F140">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G140">
         <v>3</v>
@@ -4725,13 +4725,13 @@
         </is>
       </c>
       <c r="E141">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F141">
         <v>8</v>
       </c>
       <c r="G141">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142">
@@ -4756,13 +4756,13 @@
         </is>
       </c>
       <c r="E142">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F142">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G142">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143">
@@ -4787,13 +4787,13 @@
         </is>
       </c>
       <c r="E143">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F143">
         <v>11</v>
       </c>
       <c r="G143">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144">
@@ -4818,13 +4818,13 @@
         </is>
       </c>
       <c r="E144">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F144">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G144">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145">
@@ -4849,13 +4849,13 @@
         </is>
       </c>
       <c r="E145">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F145">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G145">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146">
@@ -4883,10 +4883,10 @@
         <v>36</v>
       </c>
       <c r="F146">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G146">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="147">
@@ -4911,10 +4911,10 @@
         </is>
       </c>
       <c r="E147">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F147">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G147">
         <v>25</v>
@@ -4942,13 +4942,13 @@
         </is>
       </c>
       <c r="E148">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F148">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G148">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="149">
@@ -4973,13 +4973,13 @@
         </is>
       </c>
       <c r="E149">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F149">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G149">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150">
@@ -5004,13 +5004,13 @@
         </is>
       </c>
       <c r="E150">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F150">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G150">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="151">
@@ -5035,13 +5035,13 @@
         </is>
       </c>
       <c r="E151">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F151">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G151">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="152">
@@ -5066,13 +5066,13 @@
         </is>
       </c>
       <c r="E152">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F152">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G152">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="153">
@@ -5097,10 +5097,10 @@
         </is>
       </c>
       <c r="E153">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F153">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G153">
         <v>22</v>
@@ -5128,13 +5128,13 @@
         </is>
       </c>
       <c r="E154">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F154">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G154">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="155">
@@ -5159,13 +5159,13 @@
         </is>
       </c>
       <c r="E155">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F155">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G155">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="156">
@@ -5190,13 +5190,13 @@
         </is>
       </c>
       <c r="E156">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F156">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G156">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="157">
@@ -5221,10 +5221,10 @@
         </is>
       </c>
       <c r="E157">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F157">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G157">
         <v>16</v>
@@ -5252,10 +5252,10 @@
         </is>
       </c>
       <c r="E158">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F158">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G158">
         <v>19</v>
@@ -5283,13 +5283,13 @@
         </is>
       </c>
       <c r="E159">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F159">
         <v>11</v>
       </c>
       <c r="G159">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="160">
@@ -5314,13 +5314,13 @@
         </is>
       </c>
       <c r="E160">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F160">
         <v>10</v>
       </c>
       <c r="G160">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="161">
@@ -5345,13 +5345,13 @@
         </is>
       </c>
       <c r="E161">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F161">
         <v>13</v>
       </c>
       <c r="G161">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="162">
@@ -5376,13 +5376,13 @@
         </is>
       </c>
       <c r="E162">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F162">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G162">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="163">
@@ -5407,13 +5407,13 @@
         </is>
       </c>
       <c r="E163">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F163">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G163">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="164">
@@ -5438,13 +5438,13 @@
         </is>
       </c>
       <c r="E164">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F164">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G164">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165">
@@ -5469,13 +5469,13 @@
         </is>
       </c>
       <c r="E165">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F165">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G165">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166">
@@ -5500,10 +5500,10 @@
         </is>
       </c>
       <c r="E166">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F166">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G166">
         <v>13</v>
@@ -5531,13 +5531,13 @@
         </is>
       </c>
       <c r="E167">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F167">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G167">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="168">
@@ -5562,13 +5562,13 @@
         </is>
       </c>
       <c r="E168">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F168">
         <v>10</v>
       </c>
       <c r="G168">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169">
@@ -5593,13 +5593,13 @@
         </is>
       </c>
       <c r="E169">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F169">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G169">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170">
@@ -5624,13 +5624,13 @@
         </is>
       </c>
       <c r="E170">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F170">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G170">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="171">
@@ -5655,13 +5655,13 @@
         </is>
       </c>
       <c r="E171">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F171">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G171">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="172">
@@ -5686,13 +5686,13 @@
         </is>
       </c>
       <c r="E172">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F172">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G172">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173">
@@ -5717,13 +5717,13 @@
         </is>
       </c>
       <c r="E173">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F173">
         <v>7</v>
       </c>
       <c r="G173">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="174">
@@ -5779,13 +5779,13 @@
         </is>
       </c>
       <c r="E175">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F175">
         <v>8</v>
       </c>
       <c r="G175">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176">
@@ -5813,10 +5813,10 @@
         <v>19</v>
       </c>
       <c r="F176">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G176">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177">
@@ -5841,13 +5841,13 @@
         </is>
       </c>
       <c r="E177">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F177">
         <v>9</v>
       </c>
       <c r="G177">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178">
@@ -5875,10 +5875,10 @@
         <v>19</v>
       </c>
       <c r="F178">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G178">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179">
@@ -5903,13 +5903,13 @@
         </is>
       </c>
       <c r="E179">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F179">
         <v>8</v>
       </c>
       <c r="G179">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180">
@@ -5934,10 +5934,10 @@
         </is>
       </c>
       <c r="E180">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F180">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G180">
         <v>12</v>
@@ -5968,10 +5968,10 @@
         <v>18</v>
       </c>
       <c r="F181">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G181">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182">
@@ -5996,13 +5996,13 @@
         </is>
       </c>
       <c r="E182">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F182">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G182">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="183">
@@ -6030,10 +6030,10 @@
         <v>23</v>
       </c>
       <c r="F183">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G183">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="184">
@@ -6058,10 +6058,10 @@
         </is>
       </c>
       <c r="E184">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F184">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G184">
         <v>9</v>
@@ -6089,13 +6089,13 @@
         </is>
       </c>
       <c r="E185">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F185">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G185">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186">
@@ -6120,13 +6120,13 @@
         </is>
       </c>
       <c r="E186">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F186">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G186">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="187">
@@ -6151,13 +6151,13 @@
         </is>
       </c>
       <c r="E187">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F187">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G187">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188">
@@ -6216,10 +6216,10 @@
         <v>25</v>
       </c>
       <c r="F189">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G189">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190">
@@ -6244,13 +6244,13 @@
         </is>
       </c>
       <c r="E190">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F190">
         <v>13</v>
       </c>
       <c r="G190">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191">
@@ -6275,13 +6275,13 @@
         </is>
       </c>
       <c r="E191">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F191">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G191">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="192">
@@ -6309,10 +6309,10 @@
         <v>26</v>
       </c>
       <c r="F192">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G192">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="193">
@@ -6337,13 +6337,13 @@
         </is>
       </c>
       <c r="E193">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F193">
         <v>8</v>
       </c>
       <c r="G193">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="194">
@@ -6371,10 +6371,10 @@
         <v>24</v>
       </c>
       <c r="F194">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G194">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195">
@@ -6399,13 +6399,13 @@
         </is>
       </c>
       <c r="E195">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F195">
         <v>9</v>
       </c>
       <c r="G195">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="196">
@@ -6430,13 +6430,13 @@
         </is>
       </c>
       <c r="E196">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F196">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G196">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="197">
@@ -6461,13 +6461,13 @@
         </is>
       </c>
       <c r="E197">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F197">
         <v>9</v>
       </c>
       <c r="G197">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198">
@@ -6492,13 +6492,13 @@
         </is>
       </c>
       <c r="E198">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F198">
         <v>10</v>
       </c>
       <c r="G198">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199">
@@ -6523,13 +6523,13 @@
         </is>
       </c>
       <c r="E199">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F199">
         <v>9</v>
       </c>
       <c r="G199">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="200">
@@ -6554,13 +6554,13 @@
         </is>
       </c>
       <c r="E200">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F200">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G200">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="201">
@@ -6588,10 +6588,10 @@
         <v>43</v>
       </c>
       <c r="F201">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G201">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="202">
@@ -6619,10 +6619,10 @@
         <v>43</v>
       </c>
       <c r="F202">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G202">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="203">
@@ -6647,13 +6647,13 @@
         </is>
       </c>
       <c r="E203">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F203">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G203">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="204">
@@ -6678,13 +6678,13 @@
         </is>
       </c>
       <c r="E204">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F204">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G204">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="205">
@@ -6709,13 +6709,13 @@
         </is>
       </c>
       <c r="E205">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F205">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G205">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="206">
@@ -6740,13 +6740,13 @@
         </is>
       </c>
       <c r="E206">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F206">
+        <v>19</v>
+      </c>
+      <c r="G206">
         <v>21</v>
-      </c>
-      <c r="G206">
-        <v>23</v>
       </c>
     </row>
     <row r="207">
@@ -6771,13 +6771,13 @@
         </is>
       </c>
       <c r="E207">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F207">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G207">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="208">
@@ -6802,13 +6802,13 @@
         </is>
       </c>
       <c r="E208">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F208">
+        <v>19</v>
+      </c>
+      <c r="G208">
         <v>20</v>
-      </c>
-      <c r="G208">
-        <v>23</v>
       </c>
     </row>
     <row r="209">
@@ -6833,13 +6833,13 @@
         </is>
       </c>
       <c r="E209">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F209">
         <v>16</v>
       </c>
       <c r="G209">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="210">
@@ -6867,10 +6867,10 @@
         <v>29</v>
       </c>
       <c r="F210">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G210">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211">
@@ -6898,10 +6898,10 @@
         <v>31</v>
       </c>
       <c r="F211">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G211">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="212">
@@ -6926,10 +6926,10 @@
         </is>
       </c>
       <c r="E212">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F212">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G212">
         <v>14</v>
@@ -6957,10 +6957,10 @@
         </is>
       </c>
       <c r="E213">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F213">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G213">
         <v>15</v>
@@ -6988,13 +6988,13 @@
         </is>
       </c>
       <c r="E214">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F214">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G214">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="215">
@@ -7019,13 +7019,13 @@
         </is>
       </c>
       <c r="E215">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F215">
+        <v>16</v>
+      </c>
+      <c r="G215">
         <v>12</v>
-      </c>
-      <c r="G215">
-        <v>13</v>
       </c>
     </row>
     <row r="216">
@@ -7050,13 +7050,13 @@
         </is>
       </c>
       <c r="E216">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F216">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G216">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="217">
@@ -7081,13 +7081,13 @@
         </is>
       </c>
       <c r="E217">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F217">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G217">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="218">
@@ -7112,13 +7112,13 @@
         </is>
       </c>
       <c r="E218">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F218">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G218">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="219">
@@ -7143,13 +7143,13 @@
         </is>
       </c>
       <c r="E219">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F219">
         <v>1</v>
       </c>
       <c r="G219">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="220">
@@ -7177,10 +7177,10 @@
         <v>7</v>
       </c>
       <c r="F220">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G220">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="221">
@@ -7205,13 +7205,13 @@
         </is>
       </c>
       <c r="E221">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F221">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G221">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="222">
@@ -7236,10 +7236,10 @@
         </is>
       </c>
       <c r="E222">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F222">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G222">
         <v>7</v>
@@ -7267,13 +7267,13 @@
         </is>
       </c>
       <c r="E223">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G223">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="224">
@@ -7298,13 +7298,13 @@
         </is>
       </c>
       <c r="E224">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F224">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G224">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="225">
@@ -7329,10 +7329,10 @@
         </is>
       </c>
       <c r="E225">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F225">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G225">
         <v>6</v>
@@ -7363,10 +7363,10 @@
         <v>7</v>
       </c>
       <c r="F226">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G226">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="227">
@@ -7391,13 +7391,13 @@
         </is>
       </c>
       <c r="E227">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F227">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G227">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="228">
@@ -7422,10 +7422,10 @@
         </is>
       </c>
       <c r="E228">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F228">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G228">
         <v>15</v>
@@ -7453,13 +7453,13 @@
         </is>
       </c>
       <c r="E229">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F229">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G229">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="230">
@@ -7484,10 +7484,10 @@
         </is>
       </c>
       <c r="E230">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F230">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G230">
         <v>13</v>
@@ -7515,13 +7515,13 @@
         </is>
       </c>
       <c r="E231">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F231">
         <v>3</v>
       </c>
       <c r="G231">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="232">
@@ -7546,13 +7546,13 @@
         </is>
       </c>
       <c r="E232">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F232">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G232">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="233">
@@ -7577,13 +7577,13 @@
         </is>
       </c>
       <c r="E233">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F233">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G233">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="234">
@@ -7608,13 +7608,13 @@
         </is>
       </c>
       <c r="E234">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F234">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G234">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="235">
@@ -7639,13 +7639,13 @@
         </is>
       </c>
       <c r="E235">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F235">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G235">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>